<commit_message>
Automatische test-sync: 2025-08-05 16:19:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2</f>
+              <f>'Dashboard'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2</f>
+              <f>'Dashboard'!$B$2:$B$3</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -740,8 +740,60 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Wil je deze klant bellen?</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Testmail #1: Wil je deze klant bellen?</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Klantenservice / Contact</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar klantenservice@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-08-05 16:19:40</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2">
+  <conditionalFormatting sqref="D2:D3">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -761,7 +813,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2">
+  <conditionalFormatting sqref="G2:G3">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -769,17 +821,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2">
+  <conditionalFormatting sqref="H2:H3">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
+  <conditionalFormatting sqref="I2:I3">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2">
+  <conditionalFormatting sqref="J2:J3">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -794,7 +846,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -824,6 +876,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Klantenservice / Contact</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 16:22:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -792,8 +792,60 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Bel jij klant Jansen even?</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Testmail #2: Bel jij klant Jansen even?</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Klantenservice / Contact</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar klantenservice@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-08-05 16:22:03</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D3">
+  <conditionalFormatting sqref="D2:D4">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -813,7 +865,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G3">
+  <conditionalFormatting sqref="G2:G4">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -821,17 +873,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H3">
+  <conditionalFormatting sqref="H2:H4">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I3">
+  <conditionalFormatting sqref="I2:I4">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J3">
+  <conditionalFormatting sqref="J2:J4">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -869,17 +921,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Klantenservice / Contact</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Klantenservice / Contact</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B3" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 16:24:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$3</f>
+              <f>'Dashboard'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$3</f>
+              <f>'Dashboard'!$B$2:$B$4</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -844,8 +844,60 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Ik ben niet tevreden over hoe dit is gegaan.</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Testmail #3: Ik ben niet tevreden over hoe dit is gegaan.</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Klacht / Probleem</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar klachten@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-08-05 16:24:14</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D4">
+  <conditionalFormatting sqref="D2:D5">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -865,7 +917,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G4">
+  <conditionalFormatting sqref="G2:G5">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -873,17 +925,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H4">
+  <conditionalFormatting sqref="H2:H5">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I4">
+  <conditionalFormatting sqref="I2:I5">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J4">
+  <conditionalFormatting sqref="J2:J5">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -898,7 +950,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -938,6 +990,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Klacht / Probleem</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 16:38:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -896,8 +896,60 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Bel jij klant Jansen even?</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Testmail #1: Bel jij klant Jansen even?</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Klantenservice / Contact</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar klantenservice@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-08-05 16:37:59</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D5">
+  <conditionalFormatting sqref="D2:D6">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -917,7 +969,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G5">
+  <conditionalFormatting sqref="G2:G6">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -925,17 +977,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H5">
+  <conditionalFormatting sqref="H2:H6">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I5">
+  <conditionalFormatting sqref="I2:I6">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J5">
+  <conditionalFormatting sqref="J2:J6">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -977,7 +1029,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 16:39:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$4</f>
+              <f>'Dashboard'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$4</f>
+              <f>'Dashboard'!$B$2:$B$5</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -948,8 +948,60 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2025-08-05 16:39:02</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D6">
+  <conditionalFormatting sqref="D2:D7">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -969,7 +1021,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G6">
+  <conditionalFormatting sqref="G2:G7">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -977,17 +1029,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H6">
+  <conditionalFormatting sqref="H2:H7">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I6">
+  <conditionalFormatting sqref="I2:I7">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J6">
+  <conditionalFormatting sqref="J2:J7">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1002,7 +1054,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1052,6 +1104,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 16:46:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1000,8 +1000,60 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2025-08-05 16:46:17</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D7">
+  <conditionalFormatting sqref="D2:D8">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1021,7 +1073,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G7">
+  <conditionalFormatting sqref="G2:G8">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1029,17 +1081,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H7">
+  <conditionalFormatting sqref="H2:H8">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I7">
+  <conditionalFormatting sqref="I2:I8">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J7">
+  <conditionalFormatting sqref="J2:J8">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1087,17 +1139,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Planning / Afspraak</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Klacht / Probleem</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -1107,7 +1159,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Planning / Afspraak</t>
+          <t>Klacht / Probleem</t>
         </is>
       </c>
       <c r="B5" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 16:52:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1052,8 +1052,60 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2025-08-05 16:52:35</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D8">
+  <conditionalFormatting sqref="D2:D9">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1073,7 +1125,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G8">
+  <conditionalFormatting sqref="G2:G9">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1081,17 +1133,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H8">
+  <conditionalFormatting sqref="H2:H9">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I8">
+  <conditionalFormatting sqref="I2:I9">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J8">
+  <conditionalFormatting sqref="J2:J9">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1143,7 +1195,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 16:57:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1104,8 +1104,60 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2025-08-05 16:57:36</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D9">
+  <conditionalFormatting sqref="D2:D10">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1125,7 +1177,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G9">
+  <conditionalFormatting sqref="G2:G10">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1133,17 +1185,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H9">
+  <conditionalFormatting sqref="H2:H10">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I9">
+  <conditionalFormatting sqref="I2:I10">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J9">
+  <conditionalFormatting sqref="J2:J10">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1181,17 +1233,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Klantenservice / Contact</t>
+          <t>Planning / Afspraak</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Planning / Afspraak</t>
+          <t>Klantenservice / Contact</t>
         </is>
       </c>
       <c r="B3" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 17:01:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1156,8 +1156,60 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-08-05 17:01:06</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D10">
+  <conditionalFormatting sqref="D2:D11">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1177,7 +1229,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G10">
+  <conditionalFormatting sqref="G2:G11">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1185,17 +1237,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H10">
+  <conditionalFormatting sqref="H2:H11">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I10">
+  <conditionalFormatting sqref="I2:I11">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J10">
+  <conditionalFormatting sqref="J2:J11">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1237,7 +1289,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 17:03:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1208,8 +1208,60 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2025-08-05 17:03:26</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D11">
+  <conditionalFormatting sqref="D2:D12">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1229,7 +1281,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G11">
+  <conditionalFormatting sqref="G2:G12">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1237,17 +1289,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H11">
+  <conditionalFormatting sqref="H2:H12">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I11">
+  <conditionalFormatting sqref="I2:I12">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J11">
+  <conditionalFormatting sqref="J2:J12">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1289,7 +1341,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 17:09:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1260,8 +1260,112 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2025-08-05 17:09:08</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2025-08-05 17:09:10</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D12">
+  <conditionalFormatting sqref="D2:D14">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1281,7 +1385,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G12">
+  <conditionalFormatting sqref="G2:G14">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1289,17 +1393,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H12">
+  <conditionalFormatting sqref="H2:H14">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I12">
+  <conditionalFormatting sqref="I2:I14">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J12">
+  <conditionalFormatting sqref="J2:J14">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1341,7 +1445,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 17:15:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1364,8 +1364,60 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2025-08-05 17:15:24</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D14">
+  <conditionalFormatting sqref="D2:D15">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1385,7 +1437,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G14">
+  <conditionalFormatting sqref="G2:G15">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1393,17 +1445,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H14">
+  <conditionalFormatting sqref="H2:H15">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I14">
+  <conditionalFormatting sqref="I2:I15">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J14">
+  <conditionalFormatting sqref="J2:J15">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1445,7 +1497,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 17:18:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1416,8 +1416,60 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Wil je dit oppakken?</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Testmail #2: Wil je dit oppakken?</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2025-08-05 17:17:52</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D15">
+  <conditionalFormatting sqref="D2:D16">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1437,7 +1489,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G15">
+  <conditionalFormatting sqref="G2:G16">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1445,17 +1497,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H15">
+  <conditionalFormatting sqref="H2:H16">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I15">
+  <conditionalFormatting sqref="I2:I16">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J15">
+  <conditionalFormatting sqref="J2:J16">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1497,7 +1549,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 17:21:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1468,8 +1468,60 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2025-08-05 17:21:18</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D16">
+  <conditionalFormatting sqref="D2:D17">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1489,7 +1541,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G16">
+  <conditionalFormatting sqref="G2:G17">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1497,17 +1549,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H16">
+  <conditionalFormatting sqref="H2:H17">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I16">
+  <conditionalFormatting sqref="I2:I17">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J16">
+  <conditionalFormatting sqref="J2:J17">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1549,7 +1601,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 17:40:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1520,8 +1520,60 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2025-08-05 17:40:10</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D17">
+  <conditionalFormatting sqref="D2:D18">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1541,7 +1593,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G17">
+  <conditionalFormatting sqref="G2:G18">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1549,17 +1601,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H17">
+  <conditionalFormatting sqref="H2:H18">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I17">
+  <conditionalFormatting sqref="I2:I18">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J17">
+  <conditionalFormatting sqref="J2:J18">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1601,7 +1653,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 17:49:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1572,8 +1572,60 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2025-08-05 17:49:15</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D18">
+  <conditionalFormatting sqref="D2:D19">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1593,7 +1645,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G18">
+  <conditionalFormatting sqref="G2:G19">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1601,17 +1653,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H18">
+  <conditionalFormatting sqref="H2:H19">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I18">
+  <conditionalFormatting sqref="I2:I19">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J18">
+  <conditionalFormatting sqref="J2:J19">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1653,7 +1705,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 17:58:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1624,8 +1624,60 @@
         </is>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2025-08-05 17:57:59</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D19">
+  <conditionalFormatting sqref="D2:D20">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1645,7 +1697,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G19">
+  <conditionalFormatting sqref="G2:G20">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1653,17 +1705,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H19">
+  <conditionalFormatting sqref="H2:H20">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I19">
+  <conditionalFormatting sqref="I2:I20">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J19">
+  <conditionalFormatting sqref="J2:J20">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1705,7 +1757,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 18:04:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1676,8 +1676,60 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2025-08-05 18:04:38</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D20">
+  <conditionalFormatting sqref="D2:D21">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1697,7 +1749,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G20">
+  <conditionalFormatting sqref="G2:G21">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1705,17 +1757,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H20">
+  <conditionalFormatting sqref="H2:H21">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I20">
+  <conditionalFormatting sqref="I2:I21">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J20">
+  <conditionalFormatting sqref="J2:J21">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1757,7 +1809,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 18:06:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1728,8 +1728,60 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2025-08-05 18:06:39</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D21">
+  <conditionalFormatting sqref="D2:D22">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1749,7 +1801,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G21">
+  <conditionalFormatting sqref="G2:G22">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1757,17 +1809,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H21">
+  <conditionalFormatting sqref="H2:H22">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I21">
+  <conditionalFormatting sqref="I2:I22">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J21">
+  <conditionalFormatting sqref="J2:J22">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1809,7 +1861,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 18:08:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1780,8 +1780,60 @@
         </is>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Wil je dit oppakken?</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Testmail #2: Wil je dit oppakken?</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2025-08-05 18:08:46</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D22">
+  <conditionalFormatting sqref="D2:D23">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1801,7 +1853,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G22">
+  <conditionalFormatting sqref="G2:G23">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1809,17 +1861,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H22">
+  <conditionalFormatting sqref="H2:H23">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I22">
+  <conditionalFormatting sqref="I2:I23">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J22">
+  <conditionalFormatting sqref="J2:J23">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1861,7 +1913,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 18:11:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1832,8 +1832,60 @@
         </is>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Kun jij dit afhandelen?</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Testmail #3: Kun jij dit afhandelen?</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2025-08-05 18:10:55</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D23">
+  <conditionalFormatting sqref="D2:D24">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1853,7 +1905,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G23">
+  <conditionalFormatting sqref="G2:G24">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1861,17 +1913,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H23">
+  <conditionalFormatting sqref="H2:H24">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I23">
+  <conditionalFormatting sqref="I2:I24">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J23">
+  <conditionalFormatting sqref="J2:J24">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1913,7 +1965,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 18:13:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$5</f>
+              <f>'Dashboard'!$A$2:$A$6</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$5</f>
+              <f>'Dashboard'!$B$2:$B$6</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1884,8 +1884,60 @@
         </is>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Wil je 100 stuks M5-bouten bestellen?</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Testmail #4: Wil je 100 stuks M5-bouten bestellen?</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar inkoop@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>2025-08-05 18:13:03</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D24">
+  <conditionalFormatting sqref="D2:D25">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1905,7 +1957,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G24">
+  <conditionalFormatting sqref="G2:G25">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1913,17 +1965,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H24">
+  <conditionalFormatting sqref="H2:H25">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I24">
+  <conditionalFormatting sqref="I2:I25">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J24">
+  <conditionalFormatting sqref="J2:J25">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1938,7 +1990,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1998,6 +2050,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 18:15:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1936,8 +1936,60 @@
         </is>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Wil je deze klant bellen?</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Testmail #5: Wil je deze klant bellen?</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Klantenservice / Contact</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar klantenservice@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>2025-08-05 18:15:12</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D25">
+  <conditionalFormatting sqref="D2:D26">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1957,7 +2009,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G25">
+  <conditionalFormatting sqref="G2:G26">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1965,17 +2017,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H25">
+  <conditionalFormatting sqref="H2:H26">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I25">
+  <conditionalFormatting sqref="I2:I26">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J25">
+  <conditionalFormatting sqref="J2:J26">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2027,7 +2079,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 18:17:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1988,8 +1988,60 @@
         </is>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Hebben we EcoPro-700 nog op voorraad?</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Testmail #6: Hebben we EcoPro-700 nog op voorraad?</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar inkoop@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>2025-08-05 18:17:21</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D26">
+  <conditionalFormatting sqref="D2:D27">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2009,7 +2061,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G26">
+  <conditionalFormatting sqref="G2:G27">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2017,17 +2069,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H26">
+  <conditionalFormatting sqref="H2:H27">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I26">
+  <conditionalFormatting sqref="I2:I27">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J26">
+  <conditionalFormatting sqref="J2:J27">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2085,17 +2137,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Inkoop / Bestellingen</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Klacht / Probleem</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -2105,7 +2157,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Inkoop / Bestellingen</t>
+          <t>Klacht / Probleem</t>
         </is>
       </c>
       <c r="B6" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 18:19:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2040,8 +2040,60 @@
         </is>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Is dit artikel nog op voorraad?</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Testmail #7: Is dit artikel nog op voorraad?</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar inkoop@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>2025-08-05 18:19:30</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D27">
+  <conditionalFormatting sqref="D2:D28">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2061,7 +2113,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G27">
+  <conditionalFormatting sqref="G2:G28">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2069,17 +2121,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H27">
+  <conditionalFormatting sqref="H2:H28">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I27">
+  <conditionalFormatting sqref="I2:I28">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J27">
+  <conditionalFormatting sqref="J2:J28">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2141,7 +2193,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 18:21:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2092,8 +2092,60 @@
         </is>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Kun je nagaan of dit nog leverbaar is?</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Testmail #8: Kun je nagaan of dit nog leverbaar is?</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar inkoop@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>2025-08-05 18:21:41</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D28">
+  <conditionalFormatting sqref="D2:D29">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2113,7 +2165,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G28">
+  <conditionalFormatting sqref="G2:G29">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2121,17 +2173,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H28">
+  <conditionalFormatting sqref="H2:H29">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I28">
+  <conditionalFormatting sqref="I2:I29">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J28">
+  <conditionalFormatting sqref="J2:J29">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2179,7 +2231,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Klantenservice / Contact</t>
+          <t>Inkoop / Bestellingen</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -2189,11 +2241,11 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Inkoop / Bestellingen</t>
+          <t>Klantenservice / Contact</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 18:24:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$6</f>
+              <f>'Dashboard'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$6</f>
+              <f>'Dashboard'!$B$2:$B$7</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2144,8 +2144,60 @@
         </is>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Hoi, hebben jullie al iets gehoord?</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Testmail #9: Hoi, hebben jullie al iets gehoord?</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Opvolging / Status</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Dank voor je bericht. We hebben je eerdere e-mail ontvangen en doorgestuurd naar klantenservice@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>2025-08-05 18:23:51</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D29">
+  <conditionalFormatting sqref="D2:D30">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2165,7 +2217,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G29">
+  <conditionalFormatting sqref="G2:G30">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2173,17 +2225,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H29">
+  <conditionalFormatting sqref="H2:H30">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I29">
+  <conditionalFormatting sqref="I2:I30">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J29">
+  <conditionalFormatting sqref="J2:J30">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2198,7 +2250,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2231,7 +2283,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Inkoop / Bestellingen</t>
+          <t>Klantenservice / Contact</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -2241,7 +2293,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Klantenservice / Contact</t>
+          <t>Inkoop / Bestellingen</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -2265,6 +2317,16 @@
         </is>
       </c>
       <c r="B6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Opvolging / Status</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 18:26:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2196,8 +2196,60 @@
         </is>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Is er al nieuws?</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Testmail #10: Is er al nieuws?</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Opvolging / Status</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Dank voor je bericht. We hebben je eerdere e-mail ontvangen en doorgestuurd naar klantenservice@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>2025-08-05 18:26:02</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D30">
+  <conditionalFormatting sqref="D2:D31">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2217,7 +2269,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G30">
+  <conditionalFormatting sqref="G2:G31">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2225,17 +2277,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H30">
+  <conditionalFormatting sqref="H2:H31">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I30">
+  <conditionalFormatting sqref="I2:I31">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J30">
+  <conditionalFormatting sqref="J2:J31">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2303,17 +2355,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Opvolging / Status</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Klacht / Probleem</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -2323,7 +2375,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Opvolging / Status</t>
+          <t>Klacht / Probleem</t>
         </is>
       </c>
       <c r="B7" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 18:30:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2308,8 +2308,65 @@
         </is>
       </c>
     </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Ik heb nog geen geld terug.</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Testmail #12: Ik heb nog geen geld terug.</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw bericht. Ik begrijp dat u nog geen geld hebt ontvangen en ik help u hier graag mee verder. Om uw vraag goed te kunnen beantwoorden, zou ik wat meer informatie nodig hebben. Kunt u mij laten weten om welke transactie het gaat en eventueel het bijbehorende referentienummer? Op die manier kan ik het voor u nakijken en u verder helpen.
+Ik kijk uit naar uw reactie.
+Met vriendelijke groet,
+[Naam]
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>2025-08-05 18:30:33</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D32">
+  <conditionalFormatting sqref="D2:D33">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2329,7 +2386,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G32">
+  <conditionalFormatting sqref="G2:G33">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2337,17 +2394,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H32">
+  <conditionalFormatting sqref="H2:H33">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I32">
+  <conditionalFormatting sqref="I2:I33">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J32">
+  <conditionalFormatting sqref="J2:J33">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2419,7 +2476,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 18:33:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$7</f>
+              <f>'Dashboard'!$A$2:$A$8</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$7</f>
+              <f>'Dashboard'!$B$2:$B$8</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2365,8 +2365,60 @@
         </is>
       </c>
     </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Kun je mij de datasheet van de VentiQ-250 sturen?</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Testmail #13: Kun je mij de datasheet van de VentiQ-250 sturen?</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Documentatie / Datasheets</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar documentatie@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>2025-08-05 18:32:50</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D33">
+  <conditionalFormatting sqref="D2:D34">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2386,7 +2438,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G33">
+  <conditionalFormatting sqref="G2:G34">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2394,17 +2446,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H33">
+  <conditionalFormatting sqref="H2:H34">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I33">
+  <conditionalFormatting sqref="I2:I34">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J33">
+  <conditionalFormatting sqref="J2:J34">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2419,7 +2471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2452,7 +2504,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Klantenservice / Contact</t>
+          <t>Inkoop / Bestellingen</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -2462,7 +2514,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Inkoop / Bestellingen</t>
+          <t>Klantenservice / Contact</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -2496,6 +2548,16 @@
         </is>
       </c>
       <c r="B7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Documentatie / Datasheets</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 18:35:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$8</f>
+              <f>'Dashboard'!$A$2:$A$9</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$8</f>
+              <f>'Dashboard'!$B$2:$B$9</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2417,8 +2417,60 @@
         </is>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Heb je de CE-certificaten van dit product?</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Testmail #14: Heb je de CE-certificaten van dit product?</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Kwaliteit / Certificaten</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar kwaliteit@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>2025-08-05 18:35:01</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D34">
+  <conditionalFormatting sqref="D2:D35">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2438,7 +2490,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G34">
+  <conditionalFormatting sqref="G2:G35">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2446,17 +2498,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H34">
+  <conditionalFormatting sqref="H2:H35">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I34">
+  <conditionalFormatting sqref="I2:I35">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J34">
+  <conditionalFormatting sqref="J2:J35">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2471,7 +2523,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2504,7 +2556,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Inkoop / Bestellingen</t>
+          <t>Klantenservice / Contact</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -2514,7 +2566,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Klantenservice / Contact</t>
+          <t>Inkoop / Bestellingen</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -2558,6 +2610,16 @@
         </is>
       </c>
       <c r="B8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Kwaliteit / Certificaten</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 18:37:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2469,8 +2469,60 @@
         </is>
       </c>
     </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Leg dit even neer bij Koen.</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Testmail #15: Leg dit even neer bij Koen.</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>2025-08-05 18:37:11</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D35">
+  <conditionalFormatting sqref="D2:D36">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2490,7 +2542,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G35">
+  <conditionalFormatting sqref="G2:G36">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2498,17 +2550,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H35">
+  <conditionalFormatting sqref="H2:H36">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I35">
+  <conditionalFormatting sqref="I2:I36">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J35">
+  <conditionalFormatting sqref="J2:J36">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2550,7 +2602,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 18:39:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2521,8 +2521,60 @@
         </is>
       </c>
     </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Wil je dit even doorsturen?</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Testmail #16: Wil je dit even doorsturen?</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>2025-08-05 18:39:28</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D36">
+  <conditionalFormatting sqref="D2:D37">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2542,7 +2594,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G36">
+  <conditionalFormatting sqref="G2:G37">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2550,17 +2602,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H36">
+  <conditionalFormatting sqref="H2:H37">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I36">
+  <conditionalFormatting sqref="I2:I37">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J36">
+  <conditionalFormatting sqref="J2:J37">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2602,7 +2654,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 18:41:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2573,8 +2573,60 @@
         </is>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Testmail #17: Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>2025-08-05 18:41:37</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D37">
+  <conditionalFormatting sqref="D2:D38">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2594,7 +2646,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G37">
+  <conditionalFormatting sqref="G2:G38">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2602,17 +2654,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H37">
+  <conditionalFormatting sqref="H2:H38">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I37">
+  <conditionalFormatting sqref="I2:I38">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J37">
+  <conditionalFormatting sqref="J2:J38">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2654,7 +2706,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 18:43:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2625,8 +2625,60 @@
         </is>
       </c>
     </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Bestel je 200 stuks M8-bouten RVS voor Van Dijk?</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Testmail #18: Bestel je 200 stuks M8-bouten RVS voor Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar inkoop@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>2025-08-05 18:43:46</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D38">
+  <conditionalFormatting sqref="D2:D39">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2646,7 +2698,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G38">
+  <conditionalFormatting sqref="G2:G39">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2654,17 +2706,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H38">
+  <conditionalFormatting sqref="H2:H39">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I38">
+  <conditionalFormatting sqref="I2:I39">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J38">
+  <conditionalFormatting sqref="J2:J39">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2712,17 +2764,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Klantenservice / Contact</t>
+          <t>Inkoop / Bestellingen</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Inkoop / Bestellingen</t>
+          <t>Klantenservice / Contact</t>
         </is>
       </c>
       <c r="B4" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 18:46:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2677,8 +2677,60 @@
         </is>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Bel jij klant Jansen even?</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Testmail #19: Bel jij klant Jansen even?</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Klantenservice / Contact</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar klantenservice@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>2025-08-05 18:45:56</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D39">
+  <conditionalFormatting sqref="D2:D40">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2698,7 +2750,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G39">
+  <conditionalFormatting sqref="G2:G40">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2706,17 +2758,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H39">
+  <conditionalFormatting sqref="H2:H40">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I39">
+  <conditionalFormatting sqref="I2:I40">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J39">
+  <conditionalFormatting sqref="J2:J40">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2764,7 +2816,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Inkoop / Bestellingen</t>
+          <t>Klantenservice / Contact</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -2774,11 +2826,11 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Klantenservice / Contact</t>
+          <t>Inkoop / Bestellingen</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 18:48:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2729,8 +2729,60 @@
         </is>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Ik ben niet tevreden over hoe dit is gegaan.</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Testmail #20: Ik ben niet tevreden over hoe dit is gegaan.</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Klacht / Probleem</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar klachten@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>2025-08-05 18:48:05</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D40">
+  <conditionalFormatting sqref="D2:D41">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2750,7 +2802,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G40">
+  <conditionalFormatting sqref="G2:G41">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2758,17 +2810,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H40">
+  <conditionalFormatting sqref="H2:H41">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I40">
+  <conditionalFormatting sqref="I2:I41">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J40">
+  <conditionalFormatting sqref="J2:J41">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2846,7 +2898,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Opvolging / Status</t>
+          <t>Klacht / Probleem</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -2856,11 +2908,11 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Klacht / Probleem</t>
+          <t>Opvolging / Status</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 19:23:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2836,8 +2836,65 @@
         </is>
       </c>
     </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Kun je dit voor me fixen?</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Testmail #2: Kun je dit voor me fixen?</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Beste [naam],
+Bedankt voor je bericht. Om je beter te kunnen helpen, heb ik wat meer informatie nodig. Kun je specifiek aangeven wat er gefixt moet worden en eventueel ook wat meer details geven over het probleem dat je ervaart? Hoe meer informatie je kunt verstrekken, hoe beter we je kunnen assisteren.
+Ik zie graag je reactie tegemoet.
+Met vriendelijke groet,
+[Naam]  
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>2025-08-05 19:23:32</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D42">
+  <conditionalFormatting sqref="D2:D43">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2857,7 +2914,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G42">
+  <conditionalFormatting sqref="G2:G43">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2865,17 +2922,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H42">
+  <conditionalFormatting sqref="H2:H43">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I42">
+  <conditionalFormatting sqref="I2:I43">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J42">
+  <conditionalFormatting sqref="J2:J43">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2973,17 +3030,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Documentatie / Datasheets</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Kwaliteit / Certificaten</t>
+          <t>Documentatie / Datasheets</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -2993,7 +3050,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Overig</t>
+          <t>Kwaliteit / Certificaten</t>
         </is>
       </c>
       <c r="B10" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 19:26:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2893,8 +2893,63 @@
         </is>
       </c>
     </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Los jij dit even af?</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Testmail #3: Los jij dit even af?</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw e-mail. Het lijkt erop dat u een testmail hebt gestuurd. Als u hulp nodig heeft bij iets specifieks, laat het ons dan weten, zodat we u op de juiste manier kunnen assisteren.
+Met vriendelijke groet,
+[Naam van het bedrijf]</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>2025-08-05 19:25:51</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D43">
+  <conditionalFormatting sqref="D2:D44">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2914,7 +2969,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G43">
+  <conditionalFormatting sqref="G2:G44">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2922,17 +2977,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H43">
+  <conditionalFormatting sqref="H2:H44">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I43">
+  <conditionalFormatting sqref="I2:I44">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J43">
+  <conditionalFormatting sqref="J2:J44">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3010,17 +3065,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Klacht / Probleem</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Opvolging / Status</t>
+          <t>Klacht / Probleem</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -3030,7 +3085,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Overig</t>
+          <t>Opvolging / Status</t>
         </is>
       </c>
       <c r="B8" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 19:28:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2948,8 +2948,63 @@
         </is>
       </c>
     </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Bestel je 100 M5-bouten zodra je kan?</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Testmail #4: Bestel je 100 M5-bouten zodra je kan?</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Dank voor uw e-mail. Het lijkt erop dat u ons per abuis heeft gecontacteerd. We willen u vriendelijk verzoeken ons te voorzien van wat meer informatie, zodat we u beter van dienst kunnen zijn. Kunt u ons meer vertellen over uw specifieke behoeften en het product waar u naar op zoek bent?
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>2025-08-05 19:28:36</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D44">
+  <conditionalFormatting sqref="D2:D45">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2969,7 +3024,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G44">
+  <conditionalFormatting sqref="G2:G45">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2977,17 +3032,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H44">
+  <conditionalFormatting sqref="H2:H45">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I44">
+  <conditionalFormatting sqref="I2:I45">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J44">
+  <conditionalFormatting sqref="J2:J45">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3039,7 +3094,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 19:31:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3003,8 +3003,60 @@
         </is>
       </c>
     </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Kun jij deze klant even bellen vandaag?</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Testmail #5: Kun jij deze klant even bellen vandaag?</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar support@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>2025-08-05 19:30:54</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D45">
+  <conditionalFormatting sqref="D2:D46">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -3024,7 +3076,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G45">
+  <conditionalFormatting sqref="G2:G46">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3032,17 +3084,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H45">
+  <conditionalFormatting sqref="H2:H46">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I45">
+  <conditionalFormatting sqref="I2:I46">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J45">
+  <conditionalFormatting sqref="J2:J46">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3110,17 +3162,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Overig</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B6" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 19:33:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3055,8 +3055,63 @@
         </is>
       </c>
     </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Staan er nog EcoPro-700 op voorraad?</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Testmail #6: Staan er nog EcoPro-700 op voorraad?</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank u voor uw e-mail. Op dit moment hebben we nog EcoPro-700 op voorraad. Als u geïnteresseerd bent in het plaatsen van een bestelling, kunt u dit via onze website doen of contact opnemen met onze verkoopafdeling. Mocht u verdere vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>2025-08-05 19:33:16</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D46">
+  <conditionalFormatting sqref="D2:D47">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -3076,7 +3131,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G46">
+  <conditionalFormatting sqref="G2:G47">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3084,17 +3139,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H46">
+  <conditionalFormatting sqref="H2:H47">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I46">
+  <conditionalFormatting sqref="I2:I47">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J46">
+  <conditionalFormatting sqref="J2:J47">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3166,7 +3221,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 19:35:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3110,8 +3110,64 @@
         </is>
       </c>
     </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Is dit artikel momenteel beschikbaar?</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Testmail #7: Is dit artikel momenteel beschikbaar?</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Beste afzender,
+Hartelijk dank voor uw interesse in ons artikel. Om u nauwkeurig te kunnen informeren over de beschikbaarheid, zou u ons meer details kunnen verstrekken, zoals de naam of het artikelnummer van het gewenste product? Op basis van deze informatie kan ik voor u nagaan of het artikel momenteel op voorraad is. 
+Met vriendelijke groet,
+[Naam]
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>2025-08-05 19:35:34</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D47">
+  <conditionalFormatting sqref="D2:D48">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -3131,7 +3187,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G47">
+  <conditionalFormatting sqref="G2:G48">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3139,17 +3195,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H47">
+  <conditionalFormatting sqref="H2:H48">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I47">
+  <conditionalFormatting sqref="I2:I48">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J47">
+  <conditionalFormatting sqref="J2:J48">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3197,7 +3253,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Inkoop / Bestellingen</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -3207,17 +3263,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Klantenservice / Contact</t>
+          <t>Inkoop / Bestellingen</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Overig</t>
+          <t>Klantenservice / Contact</t>
         </is>
       </c>
       <c r="B5" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 19:38:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J48"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3166,8 +3166,67 @@
         </is>
       </c>
     </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Check jij even of dit nog geleverd kan worden?</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Testmail #8: Check jij even of dit nog geleverd kan worden?</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank u voor uw e-mail. Om uw vraag over de levering te beantwoorden, hebben we wat meer informatie nodig. Kunt u ons alstublieft het volgende verstrekken:
+- Het specifieke product dat u wilt bestellen
+- Het afleveradres
+- Gewenste leverdatum
+Met deze informatie kunnen we controleren of het product nog steeds geleverd kan worden. We kijken uit naar uw antwoord.
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>2025-08-05 19:37:52</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D48">
+  <conditionalFormatting sqref="D2:D49">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -3187,7 +3246,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G48">
+  <conditionalFormatting sqref="G2:G49">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3195,17 +3254,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H48">
+  <conditionalFormatting sqref="H2:H49">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I48">
+  <conditionalFormatting sqref="I2:I49">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J48">
+  <conditionalFormatting sqref="J2:J49">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3257,7 +3316,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 19:40:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3225,8 +3225,60 @@
         </is>
       </c>
     </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Hebben jullie toevallig al iets gehoord?</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Testmail #9: Hebben jullie toevallig al iets gehoord?</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar support@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>2025-08-05 19:40:09</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D49">
+  <conditionalFormatting sqref="D2:D50">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -3246,7 +3298,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G49">
+  <conditionalFormatting sqref="G2:G50">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3254,17 +3306,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H49">
+  <conditionalFormatting sqref="H2:H50">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I49">
+  <conditionalFormatting sqref="I2:I50">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J49">
+  <conditionalFormatting sqref="J2:J50">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3316,7 +3368,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 19:42:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3277,8 +3277,60 @@
         </is>
       </c>
     </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Laat maar weten of er nieuws is</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Testmail #10: Laat maar weten of er nieuws is</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar support@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>2025-08-05 19:42:19</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D50">
+  <conditionalFormatting sqref="D2:D51">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -3298,7 +3350,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G50">
+  <conditionalFormatting sqref="G2:G51">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3306,17 +3358,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H50">
+  <conditionalFormatting sqref="H2:H51">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I50">
+  <conditionalFormatting sqref="I2:I51">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J50">
+  <conditionalFormatting sqref="J2:J51">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3368,7 +3420,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 19:44:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J51"/>
+  <dimension ref="A1:J52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3329,8 +3329,64 @@
         </is>
       </c>
     </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Weten jullie al iets over mijn retour?</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Testmail #11: Weten jullie al iets over mijn retour?</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor je e-mail. Om je vraag over je retour te kunnen beantwoorden, hebben we wat meer informatie nodig. Zou je ons alsjeblieft je ordernummer en/of trackingnummer kunnen geven? Hiermee kunnen we het proces van je retourzending bekijken en je van de juiste informatie voorzien.
+Alvast bedankt voor je medewerking.
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>2025-08-05 19:44:30</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D51">
+  <conditionalFormatting sqref="D2:D52">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -3350,7 +3406,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G51">
+  <conditionalFormatting sqref="G2:G52">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3358,17 +3414,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H51">
+  <conditionalFormatting sqref="H2:H52">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I51">
+  <conditionalFormatting sqref="I2:I52">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J51">
+  <conditionalFormatting sqref="J2:J52">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3450,7 +3506,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 19:47:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J52"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3385,8 +3385,63 @@
         </is>
       </c>
     </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Wanneer wordt het geld van mijn retour overgemaakt?</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Testmail #12: Wanneer wordt het geld van mijn retour overgemaakt?</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Dank u voor uw e-mail. Om uw terugbetaling te kunnen verwerken en het geld over te maken, hebben wij wat meer informatie nodig. Kunt u ons alstublieft uw ordernummer en de naam waaronder de bestelling geplaatst is, doorgeven? Zodra we deze gegevens ontvangen hebben, zullen we het proces voor de terugbetaling in gang zetten.
+Met vriendelijke groet,
+[Naam bedrijf] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>2025-08-05 19:47:12</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D52">
+  <conditionalFormatting sqref="D2:D53">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -3406,7 +3461,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G52">
+  <conditionalFormatting sqref="G2:G53">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3414,17 +3469,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H52">
+  <conditionalFormatting sqref="H2:H53">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I52">
+  <conditionalFormatting sqref="I2:I53">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J52">
+  <conditionalFormatting sqref="J2:J53">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3492,7 +3547,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Klantenservice / Contact</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -3502,11 +3557,11 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Klantenservice / Contact</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 19:49:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J53"/>
+  <dimension ref="A1:J54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3440,8 +3440,60 @@
         </is>
       </c>
     </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Stuur je me even de datasheet van VentiQ-250?</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Testmail #13: Stuur je me even de datasheet van VentiQ-250?</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Documentatie / Datasheets</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar documentatie@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>2025-08-05 19:49:27</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D53">
+  <conditionalFormatting sqref="D2:D54">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -3461,7 +3513,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G53">
+  <conditionalFormatting sqref="G2:G54">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3469,17 +3521,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H53">
+  <conditionalFormatting sqref="H2:H54">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I53">
+  <conditionalFormatting sqref="I2:I54">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J53">
+  <conditionalFormatting sqref="J2:J54">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3591,7 +3643,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 19:51:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:J55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3492,8 +3492,60 @@
         </is>
       </c>
     </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Heb je ergens de CE-certificaten van dit product?</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Testmail #14: Heb je ergens de CE-certificaten van dit product?</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Kwaliteit / Certificaten</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar kwaliteit@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>2025-08-05 19:51:36</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D54">
+  <conditionalFormatting sqref="D2:D55">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -3513,7 +3565,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G54">
+  <conditionalFormatting sqref="G2:G55">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3521,17 +3573,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H54">
+  <conditionalFormatting sqref="H2:H55">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I54">
+  <conditionalFormatting sqref="I2:I55">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J54">
+  <conditionalFormatting sqref="J2:J55">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3653,7 +3705,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 19:54:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J55"/>
+  <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3544,8 +3544,64 @@
         </is>
       </c>
     </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Wil je dit even bij Koen neerleggen?</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Testmail #15: Wil je dit even bij Koen neerleggen?</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Beste heer/mevrouw,
+Bedankt voor uw e-mail. Kunt u specifieker aangeven wat u precies bij Koen neergelegd wilt hebben? Zo kan ik ervoor zorgen dat uw verzoek correct wordt afgehandeld.
+Met vriendelijke groet,
+[Naam] 
+E-mailassistent van [Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>2025-08-05 19:53:45</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D55">
+  <conditionalFormatting sqref="D2:D56">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -3565,7 +3621,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G55">
+  <conditionalFormatting sqref="G2:G56">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3573,17 +3629,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H55">
+  <conditionalFormatting sqref="H2:H56">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I55">
+  <conditionalFormatting sqref="I2:I56">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J55">
+  <conditionalFormatting sqref="J2:J56">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3635,7 +3691,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 19:56:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J56"/>
+  <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3600,8 +3600,63 @@
         </is>
       </c>
     </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Zou je dit kunnen doorsturen?</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Testmail #16: Zou je dit kunnen doorsturen?</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Hartelijk dank voor uw e-mail. Om u beter van dienst te kunnen zijn, zou u ons meer informatie kunnen geven over wat u precies wilt laten doorsturen? Op die manier kunnen we u gerichter helpen.
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>2025-08-05 19:56:03</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D56">
+  <conditionalFormatting sqref="D2:D57">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -3621,7 +3676,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G56">
+  <conditionalFormatting sqref="G2:G57">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3629,17 +3684,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H56">
+  <conditionalFormatting sqref="H2:H57">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I56">
+  <conditionalFormatting sqref="I2:I57">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J56">
+  <conditionalFormatting sqref="J2:J57">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3691,7 +3746,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 19:58:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J57"/>
+  <dimension ref="A1:J58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3655,8 +3655,63 @@
         </is>
       </c>
     </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Plan jij vrijdag om 11:00 die demo bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Testmail #17: Plan jij vrijdag om 11:00 die demo bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Geachte heer/mevrouw,
+Bedankt voor uw e-mail. Dit lijkt op een testmail. Als u een demo bij Van Dijk wilt plannen, kunt u contact met ons opnemen via de juiste kanalen om een afspraak te maken.
+Met vriendelijke groet,
+[Naam] Bedrijfsnaam [Contactgegevens]</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>2025-08-05 19:58:22</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D57">
+  <conditionalFormatting sqref="D2:D58">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -3676,7 +3731,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G57">
+  <conditionalFormatting sqref="G2:G58">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3684,17 +3739,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H57">
+  <conditionalFormatting sqref="H2:H58">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I57">
+  <conditionalFormatting sqref="I2:I58">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J57">
+  <conditionalFormatting sqref="J2:J58">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3746,7 +3801,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 20:00:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J58"/>
+  <dimension ref="A1:J59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3710,8 +3710,63 @@
         </is>
       </c>
     </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Kun je 200 M8-bouten RVS bestellen voor Van Dijk?</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Testmail #18: Kun je 200 M8-bouten RVS bestellen voor Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw e-mail. Om uw verzoek te kunnen verwerken, hebben we wat meer informatie nodig. Kunt u ons misschien laten weten van welke leverancier u de M8-bouten RVS wilt bestellen en wat het gewenste aantal is? Op die manier kunnen we uw bestelling nauwkeurig verwerken.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>2025-08-05 20:00:40</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D58">
+  <conditionalFormatting sqref="D2:D59">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -3731,7 +3786,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G58">
+  <conditionalFormatting sqref="G2:G59">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3739,17 +3794,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H58">
+  <conditionalFormatting sqref="H2:H59">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I58">
+  <conditionalFormatting sqref="I2:I59">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J58">
+  <conditionalFormatting sqref="J2:J59">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3811,7 +3866,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 20:03:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J59"/>
+  <dimension ref="A1:J60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3765,8 +3765,60 @@
         </is>
       </c>
     </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Zou jij klant Jansen nog kunnen bellen?</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Testmail #19: Zou jij klant Jansen nog kunnen bellen?</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar support@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>2025-08-05 20:03:03</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D59">
+  <conditionalFormatting sqref="D2:D60">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -3786,7 +3838,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G59">
+  <conditionalFormatting sqref="G2:G60">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3794,17 +3846,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H59">
+  <conditionalFormatting sqref="H2:H60">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I59">
+  <conditionalFormatting sqref="I2:I60">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J59">
+  <conditionalFormatting sqref="J2:J60">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3856,7 +3908,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-05 20:05:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-05.xlsx
+++ b/logs/mail_log_2025-08-05.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J60"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3817,8 +3817,64 @@
         </is>
       </c>
     </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Dit is echt niet netjes verlopen zo</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Testmail #20: Dit is echt niet netjes verlopen zo</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw bericht. Kunt u wat meer details geven over wat er precies niet netjes is verlopen? Met deze informatie kunnen we het probleem beter begrijpen en u een passende oplossing bieden.
+Met vriendelijke groet,
+[Naam]
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>2025-08-05 20:05:12</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D60">
+  <conditionalFormatting sqref="D2:D61">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -3838,7 +3894,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G60">
+  <conditionalFormatting sqref="G2:G61">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3846,17 +3902,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H60">
+  <conditionalFormatting sqref="H2:H61">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I60">
+  <conditionalFormatting sqref="I2:I61">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J60">
+  <conditionalFormatting sqref="J2:J61">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3908,7 +3964,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">

</xml_diff>